<commit_message>
matlab scripts to properly process and analyze JND data
</commit_message>
<xml_diff>
--- a/JND_Study/JND_Data/3-5-24.xlsx
+++ b/JND_Study/JND_Data/3-5-24.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Sreela/Documents/School/Stanford/Year3_2/PIEZO2/JND_Study/JND_Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2551DE4-E459-9042-9E4B-ED181C46AE39}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A33FB5AA-F796-754F-B039-4BCC35EE003C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="45300" yWindow="180" windowWidth="43320" windowHeight="24120" activeTab="1" xr2:uid="{25D944B7-559C-0549-BC33-C06F5F515E2F}"/>
+    <workbookView xWindow="38120" yWindow="180" windowWidth="43320" windowHeight="24120" activeTab="1" xr2:uid="{25D944B7-559C-0549-BC33-C06F5F515E2F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
     <definedName name="bloop2_1" localSheetId="0">Sheet1!$A$1:$H$19</definedName>
     <definedName name="bloop3" localSheetId="1">Sheet2!$A$1:$L$19</definedName>
   </definedNames>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -43,7 +43,7 @@
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
 <connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16">
   <connection id="1" xr16:uid="{583E01A4-B3C7-5E45-93F6-9AAAFD6AF031}" name="bloop2" type="6" refreshedVersion="8" background="1" saveData="1">
-    <textPr codePage="10000" sourceFile="/Users/Sreela/Documents/School/Stanford/Year3_2/PIEZO2/JND_Study/JND_Data/bloop2.csv" comma="1">
+    <textPr sourceFile="/Users/Sreela/Documents/School/Stanford/Year3_2/PIEZO2/JND_Study/JND_Data/bloop2.csv" comma="1">
       <textFields count="8">
         <textField/>
         <textField/>
@@ -57,7 +57,7 @@
     </textPr>
   </connection>
   <connection id="2" xr16:uid="{6FD93F8A-E595-7D43-94B5-A22C512FD7CB}" name="bloop3" type="6" refreshedVersion="8" background="1" saveData="1">
-    <textPr codePage="10000" sourceFile="/Users/Sreela/Documents/School/Stanford/Year3_2/PIEZO2/JND_Study/JND_Data/bloop3.csv" comma="1">
+    <textPr sourceFile="/Users/Sreela/Documents/School/Stanford/Year3_2/PIEZO2/JND_Study/JND_Data/bloop3.csv" comma="1">
       <textFields count="8">
         <textField/>
         <textField/>
@@ -1329,9 +1329,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1369,7 +1369,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1475,7 +1475,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1617,7 +1617,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2065,8 +2065,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{45FCDB44-A1A8-744B-A881-1B84EA32A9A2}">
   <dimension ref="A1:M27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="E32" sqref="E32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2130,7 +2130,7 @@
         <v>67</v>
       </c>
       <c r="C2">
-        <f>(B2-$C$25)*($D$27-$D$25)/($C$27-$C$25)</f>
+        <f t="shared" ref="C2:C19" si="0">(B2-$C$25)*($D$27-$D$25)/($C$27-$C$25)</f>
         <v>4.3478260869565215</v>
       </c>
       <c r="D2">
@@ -2176,28 +2176,28 @@
         <v>94</v>
       </c>
       <c r="C3">
-        <f>(B3-$C$25)*($D$27-$D$25)/($C$27-$C$25)</f>
+        <f t="shared" si="0"/>
         <v>10.217391304347826</v>
       </c>
       <c r="D3">
         <v>646.52499999999998</v>
       </c>
       <c r="E3">
-        <f t="shared" ref="E3:E19" si="0">(D3-$E$25) * $D$27 / ($E$27-$E$25)</f>
+        <f t="shared" ref="E3:E19" si="1">(D3-$E$25) * $D$27 / ($E$27-$E$25)</f>
         <v>7.6963636363636363</v>
       </c>
       <c r="F3">
         <v>48.190760265843402</v>
       </c>
       <c r="G3">
-        <f t="shared" ref="G3:G19" si="1">F3*$D$26/($E$25-$E$26)</f>
+        <f t="shared" ref="G3:G19" si="2">F3*$D$26/($E$25-$E$26)</f>
         <v>1.1684240198534099</v>
       </c>
       <c r="H3">
         <v>40</v>
       </c>
       <c r="I3">
-        <f t="shared" ref="I3:I19" si="2">G3/SQRT(H3)</f>
+        <f t="shared" ref="I3:I19" si="3">G3/SQRT(H3)</f>
         <v>0.18474405877932865</v>
       </c>
       <c r="J3">
@@ -2210,7 +2210,7 @@
         <v>40</v>
       </c>
       <c r="M3">
-        <f t="shared" ref="M3:M19" si="3">K3/SQRT(L3)</f>
+        <f t="shared" ref="M3:M19" si="4">K3/SQRT(L3)</f>
         <v>0.13535600628527708</v>
       </c>
     </row>
@@ -2222,28 +2222,28 @@
         <v>95</v>
       </c>
       <c r="C4">
-        <f>(B4-$C$25)*($D$27-$D$25)/($C$27-$C$25)</f>
+        <f t="shared" si="0"/>
         <v>10.434782608695652</v>
       </c>
       <c r="D4">
         <v>635.967961165048</v>
       </c>
       <c r="E4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>7.9522918505442908</v>
       </c>
       <c r="F4">
         <v>46.704939789036402</v>
       </c>
       <c r="G4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1.1323990987956312</v>
       </c>
       <c r="H4">
         <v>1030</v>
       </c>
       <c r="I4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>3.5284250989863548E-2</v>
       </c>
       <c r="J4">
@@ -2256,7 +2256,7 @@
         <v>1030</v>
       </c>
       <c r="M4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>2.6036016713066309E-2</v>
       </c>
     </row>
@@ -2268,28 +2268,28 @@
         <v>96</v>
       </c>
       <c r="C5">
-        <f>(B5-$C$25)*($D$27-$D$25)/($C$27-$C$25)</f>
+        <f t="shared" si="0"/>
         <v>10.652173913043478</v>
       </c>
       <c r="D5">
         <v>630.51666666666597</v>
       </c>
       <c r="E5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>8.0844444444444612</v>
       </c>
       <c r="F5">
         <v>52.986001820187198</v>
       </c>
       <c r="G5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1.2846885357520248</v>
       </c>
       <c r="H5">
         <v>60</v>
       </c>
       <c r="I5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.16585257680103946</v>
       </c>
       <c r="J5">
@@ -2302,7 +2302,7 @@
         <v>60</v>
       </c>
       <c r="M5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.12980491059591978</v>
       </c>
     </row>
@@ -2314,28 +2314,28 @@
         <v>97</v>
       </c>
       <c r="C6">
-        <f>(B6-$C$25)*($D$27-$D$25)/($C$27-$C$25)</f>
+        <f t="shared" si="0"/>
         <v>10.869565217391305</v>
       </c>
       <c r="D6">
         <v>624.04999999999995</v>
       </c>
       <c r="E6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>8.2412121212121221</v>
       </c>
       <c r="F6">
         <v>53.410368843512003</v>
       </c>
       <c r="G6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1.2949776579935313</v>
       </c>
       <c r="H6">
         <v>100</v>
       </c>
       <c r="I6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.12949776579935313</v>
       </c>
       <c r="J6">
@@ -2348,7 +2348,7 @@
         <v>100</v>
       </c>
       <c r="M6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>9.8541773375558805E-2</v>
       </c>
     </row>
@@ -2360,28 +2360,28 @@
         <v>98</v>
       </c>
       <c r="C7">
-        <f>(B7-$C$25)*($D$27-$D$25)/($C$27-$C$25)</f>
+        <f t="shared" si="0"/>
         <v>11.086956521739131</v>
       </c>
       <c r="D7">
         <v>618.579831932773</v>
       </c>
       <c r="E7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>8.3738222561752007</v>
       </c>
       <c r="F7">
         <v>50.816773482764901</v>
       </c>
       <c r="G7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1.2320938375150821</v>
       </c>
       <c r="H7">
         <v>119</v>
       </c>
       <c r="I7">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.11294585690477969</v>
       </c>
       <c r="J7">
@@ -2394,7 +2394,7 @@
         <v>119</v>
       </c>
       <c r="M7">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>8.802963782833112E-2</v>
       </c>
     </row>
@@ -2406,28 +2406,28 @@
         <v>99</v>
       </c>
       <c r="C8">
-        <f>(B8-$C$25)*($D$27-$D$25)/($C$27-$C$25)</f>
+        <f t="shared" si="0"/>
         <v>11.304347826086957</v>
       </c>
       <c r="D8">
         <v>610.231884057971</v>
       </c>
       <c r="E8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>8.5761967501097942</v>
       </c>
       <c r="F8">
         <v>56.483971030787501</v>
       </c>
       <c r="G8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1.369499632813507</v>
       </c>
       <c r="H8">
         <v>138</v>
       </c>
       <c r="I8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.11657955063042061</v>
       </c>
       <c r="J8">
@@ -2440,7 +2440,7 @@
         <v>138</v>
       </c>
       <c r="M8">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>8.8947437066350984E-2</v>
       </c>
     </row>
@@ -2452,28 +2452,28 @@
         <v>100</v>
       </c>
       <c r="C9">
-        <f>(B9-$C$25)*($D$27-$D$25)/($C$27-$C$25)</f>
+        <f t="shared" si="0"/>
         <v>11.521739130434783</v>
       </c>
       <c r="D9">
         <v>603.38655462184795</v>
       </c>
       <c r="E9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>8.7421441303794438</v>
       </c>
       <c r="F9">
         <v>58.889457652309403</v>
       </c>
       <c r="G9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1.4278226045308535</v>
       </c>
       <c r="H9">
         <v>119</v>
       </c>
       <c r="I9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.13088828355963397</v>
       </c>
       <c r="J9">
@@ -2486,7 +2486,7 @@
         <v>119</v>
       </c>
       <c r="M9">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>9.9851014637595867E-2</v>
       </c>
     </row>
@@ -2498,28 +2498,28 @@
         <v>101</v>
       </c>
       <c r="C10">
-        <f>(B10-$C$25)*($D$27-$D$25)/($C$27-$C$25)</f>
+        <f t="shared" si="0"/>
         <v>11.739130434782609</v>
       </c>
       <c r="D10">
         <v>594.42857142857099</v>
       </c>
       <c r="E10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>8.9593073593073687</v>
       </c>
       <c r="F10">
         <v>56.5588221247937</v>
       </c>
       <c r="G10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1.3713144582212551</v>
       </c>
       <c r="H10">
         <v>119</v>
       </c>
       <c r="I10">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.12570819028044805</v>
       </c>
       <c r="J10">
@@ -2532,7 +2532,7 @@
         <v>119</v>
       </c>
       <c r="M10">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.10019389519287072</v>
       </c>
     </row>
@@ -2544,28 +2544,28 @@
         <v>102</v>
       </c>
       <c r="C11">
-        <f>(B11-$C$25)*($D$27-$D$25)/($C$27-$C$25)</f>
+        <f t="shared" si="0"/>
         <v>11.956521739130435</v>
       </c>
       <c r="D11">
         <v>586.57627118643995</v>
       </c>
       <c r="E11">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>9.1496661530560015</v>
       </c>
       <c r="F11">
         <v>64.461577937277795</v>
       </c>
       <c r="G11">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1.5629231745686347</v>
       </c>
       <c r="H11">
         <v>59</v>
       </c>
       <c r="I11">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.20347526604378263</v>
       </c>
       <c r="J11">
@@ -2578,7 +2578,7 @@
         <v>59</v>
       </c>
       <c r="M11">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.15644409689123837</v>
       </c>
     </row>
@@ -2590,28 +2590,28 @@
         <v>103</v>
       </c>
       <c r="C12">
-        <f>(B12-$C$25)*($D$27-$D$25)/($C$27-$C$25)</f>
+        <f t="shared" si="0"/>
         <v>12.173913043478262</v>
       </c>
       <c r="D12">
         <v>579.5</v>
       </c>
       <c r="E12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>9.3212121212121204</v>
       </c>
       <c r="F12">
         <v>70.359789652897604</v>
       </c>
       <c r="G12">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1.7059300954948358</v>
       </c>
       <c r="H12">
         <v>40</v>
       </c>
       <c r="I12">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.26973123153961143</v>
       </c>
       <c r="J12">
@@ -2624,7 +2624,7 @@
         <v>40</v>
       </c>
       <c r="M12">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.21311968101866963</v>
       </c>
     </row>
@@ -2636,28 +2636,28 @@
         <v>104</v>
       </c>
       <c r="C13">
-        <f>(B13-$C$25)*($D$27-$D$25)/($C$27-$C$25)</f>
+        <f t="shared" si="0"/>
         <v>12.391304347826088</v>
       </c>
       <c r="D13">
         <v>575.54999999999995</v>
       </c>
       <c r="E13">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>9.4169696969696979</v>
       </c>
       <c r="F13">
         <v>68.355669113834296</v>
       </c>
       <c r="G13">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1.6573385695756471</v>
       </c>
       <c r="H13">
         <v>40</v>
       </c>
       <c r="I13">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.26204823669522426</v>
       </c>
       <c r="J13">
@@ -2670,7 +2670,7 @@
         <v>40</v>
       </c>
       <c r="M13">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.21415128633164879</v>
       </c>
     </row>
@@ -2682,28 +2682,28 @@
         <v>105</v>
       </c>
       <c r="C14">
-        <f>(B14-$C$25)*($D$27-$D$25)/($C$27-$C$25)</f>
+        <f t="shared" si="0"/>
         <v>12.608695652173912</v>
       </c>
       <c r="D14">
         <v>561.6</v>
       </c>
       <c r="E14">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>9.7551515151515158</v>
       </c>
       <c r="F14">
         <v>77.1747367990328</v>
       </c>
       <c r="G14">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1.8711640095407953</v>
       </c>
       <c r="H14">
         <v>20</v>
       </c>
       <c r="I14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.41840499223842831</v>
       </c>
       <c r="J14">
@@ -2716,7 +2716,7 @@
         <v>20</v>
       </c>
       <c r="M14">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.31807750627794895</v>
       </c>
     </row>
@@ -2728,28 +2728,28 @@
         <v>108</v>
       </c>
       <c r="C15">
-        <f>(B15-$C$25)*($D$27-$D$25)/($C$27-$C$25)</f>
+        <f t="shared" si="0"/>
         <v>13.260869565217391</v>
       </c>
       <c r="D15">
         <v>526.75</v>
       </c>
       <c r="E15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>10.6</v>
       </c>
       <c r="F15">
         <v>91.853619961327595</v>
       </c>
       <c r="G15">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2.2270654225260436</v>
       </c>
       <c r="H15">
         <v>20</v>
       </c>
       <c r="I15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.49798696751075244</v>
       </c>
       <c r="J15">
@@ -2762,7 +2762,7 @@
         <v>20</v>
       </c>
       <c r="M15">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.34929104984238946</v>
       </c>
     </row>
@@ -2774,28 +2774,28 @@
         <v>111</v>
       </c>
       <c r="C16">
-        <f>(B16-$C$25)*($D$27-$D$25)/($C$27-$C$25)</f>
+        <f t="shared" si="0"/>
         <v>13.913043478260869</v>
       </c>
       <c r="D16">
         <v>504.1</v>
       </c>
       <c r="E16">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>11.149090909090908</v>
       </c>
       <c r="F16">
         <v>102.372310709488</v>
       </c>
       <c r="G16">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2.4820996004423348</v>
       </c>
       <c r="H16">
         <v>20</v>
       </c>
       <c r="I16">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.55501434335141275</v>
       </c>
       <c r="J16">
@@ -2808,7 +2808,7 @@
         <v>20</v>
       </c>
       <c r="M16">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.38686754839350201</v>
       </c>
     </row>
@@ -2820,28 +2820,28 @@
         <v>114</v>
       </c>
       <c r="C17">
-        <f>(B17-$C$25)*($D$27-$D$25)/($C$27-$C$25)</f>
+        <f t="shared" si="0"/>
         <v>14.565217391304348</v>
       </c>
       <c r="D17">
         <v>492.55</v>
       </c>
       <c r="E17">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>11.42909090909091</v>
       </c>
       <c r="F17">
         <v>93.820826579176895</v>
       </c>
       <c r="G17">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2.2747619405230597</v>
       </c>
       <c r="H17">
         <v>20</v>
       </c>
       <c r="I17">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.50865223316388952</v>
       </c>
       <c r="J17">
@@ -2854,7 +2854,7 @@
         <v>20</v>
       </c>
       <c r="M17">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.38540731700371172</v>
       </c>
     </row>
@@ -2866,28 +2866,28 @@
         <v>117</v>
       </c>
       <c r="C18">
-        <f>(B18-$C$25)*($D$27-$D$25)/($C$27-$C$25)</f>
+        <f t="shared" si="0"/>
         <v>15.217391304347826</v>
       </c>
       <c r="D18">
         <v>461.05</v>
       </c>
       <c r="E18">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>12.192727272727273</v>
       </c>
       <c r="F18">
         <v>88.594285933123203</v>
       </c>
       <c r="G18">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2.1480402287695792</v>
       </c>
       <c r="H18">
         <v>20</v>
       </c>
       <c r="I18">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.48031639699329781</v>
       </c>
       <c r="J18">
@@ -2900,7 +2900,7 @@
         <v>20</v>
       </c>
       <c r="M18">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.36362705826161829</v>
       </c>
     </row>
@@ -2912,28 +2912,28 @@
         <v>120</v>
       </c>
       <c r="C19">
-        <f>(B19-$C$25)*($D$27-$D$25)/($C$27-$C$25)</f>
+        <f t="shared" si="0"/>
         <v>15.869565217391305</v>
       </c>
       <c r="D19">
         <v>461.25</v>
       </c>
       <c r="E19">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>12.187878787878788</v>
       </c>
       <c r="F19">
         <v>107.87023454132201</v>
       </c>
       <c r="G19">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2.6154012173706005</v>
       </c>
       <c r="H19">
         <v>20</v>
       </c>
       <c r="I19">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.58482149104763659</v>
       </c>
       <c r="J19">
@@ -2946,7 +2946,7 @@
         <v>20</v>
       </c>
       <c r="M19">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.45827098969932428</v>
       </c>
     </row>

</xml_diff>